<commit_message>
Finished prototype TrackModel functionality
</commit_message>
<xml_diff>
--- a/TrainProject/Excel Files/TrackLayout.xlsx
+++ b/TrainProject/Excel Files/TrackLayout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="86">
   <si>
     <t>Block Number</t>
   </si>
@@ -701,8 +701,8 @@
   <dimension ref="A1:L154"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <pane ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:L78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -713,7 +713,7 @@
     <col min="4" max="4" width="11" style="3" customWidth="1"/>
     <col min="5" max="5" width="10.5703125" style="3" customWidth="1"/>
     <col min="6" max="6" width="13.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.42578125" style="3" customWidth="1"/>
     <col min="8" max="10" width="8.85546875" style="1"/>
     <col min="11" max="11" width="10.7109375" style="3" customWidth="1"/>
     <col min="12" max="12" width="11.28515625" style="3" customWidth="1"/>
@@ -3524,11 +3524,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L153"/>
+  <dimension ref="A1:L230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A154" sqref="A154:XFD154"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E169" sqref="E169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8394,6 +8394,2538 @@
         <v>83</v>
       </c>
     </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C154" s="5">
+        <v>1</v>
+      </c>
+      <c r="D154" s="3">
+        <v>50</v>
+      </c>
+      <c r="E154" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F154" s="3">
+        <v>40</v>
+      </c>
+      <c r="I154" s="8">
+        <f>E154*D154/100</f>
+        <v>0.25</v>
+      </c>
+      <c r="J154" s="8">
+        <f>I154</f>
+        <v>0.25</v>
+      </c>
+      <c r="K154" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L154" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="str">
+        <f>A154</f>
+        <v>Red</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C155" s="3">
+        <v>2</v>
+      </c>
+      <c r="D155" s="3">
+        <v>50</v>
+      </c>
+      <c r="E155" s="3">
+        <v>1</v>
+      </c>
+      <c r="F155" s="3">
+        <v>40</v>
+      </c>
+      <c r="I155" s="8">
+        <f t="shared" ref="I155:I218" si="13">E155*D155/100</f>
+        <v>0.5</v>
+      </c>
+      <c r="J155" s="8">
+        <f>I155+J154</f>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="str">
+        <f t="shared" ref="A156:A219" si="14">A155</f>
+        <v>Red</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C156" s="3">
+        <v>3</v>
+      </c>
+      <c r="D156" s="3">
+        <v>50</v>
+      </c>
+      <c r="E156" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F156" s="3">
+        <v>40</v>
+      </c>
+      <c r="I156" s="8">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="J156" s="8">
+        <f t="shared" ref="J156:J219" si="15">I156+J155</f>
+        <v>1.5</v>
+      </c>
+      <c r="L156" s="5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C157" s="5">
+        <v>4</v>
+      </c>
+      <c r="D157" s="3">
+        <v>50</v>
+      </c>
+      <c r="E157" s="3">
+        <v>2</v>
+      </c>
+      <c r="F157" s="3">
+        <v>40</v>
+      </c>
+      <c r="I157" s="8">
+        <f t="shared" si="13"/>
+        <v>1</v>
+      </c>
+      <c r="J157" s="8">
+        <f t="shared" si="15"/>
+        <v>2.5</v>
+      </c>
+      <c r="L157" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C158" s="3">
+        <v>5</v>
+      </c>
+      <c r="D158" s="3">
+        <v>50</v>
+      </c>
+      <c r="E158" s="3">
+        <v>1.5</v>
+      </c>
+      <c r="F158" s="3">
+        <v>40</v>
+      </c>
+      <c r="I158" s="8">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="J158" s="8">
+        <f t="shared" si="15"/>
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A159" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C159" s="3">
+        <v>6</v>
+      </c>
+      <c r="D159" s="3">
+        <v>50</v>
+      </c>
+      <c r="E159" s="3">
+        <v>1</v>
+      </c>
+      <c r="F159" s="3">
+        <v>40</v>
+      </c>
+      <c r="I159" s="8">
+        <f t="shared" si="13"/>
+        <v>0.5</v>
+      </c>
+      <c r="J159" s="8">
+        <f t="shared" si="15"/>
+        <v>3.75</v>
+      </c>
+      <c r="L159" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A160" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C160" s="5">
+        <v>7</v>
+      </c>
+      <c r="D160" s="3">
+        <v>75</v>
+      </c>
+      <c r="E160" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F160" s="3">
+        <v>40</v>
+      </c>
+      <c r="G160" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="I160" s="8">
+        <f t="shared" si="13"/>
+        <v>0.375</v>
+      </c>
+      <c r="J160" s="8">
+        <f t="shared" si="15"/>
+        <v>4.125</v>
+      </c>
+      <c r="L160" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C161" s="3">
+        <v>8</v>
+      </c>
+      <c r="D161" s="3">
+        <v>75</v>
+      </c>
+      <c r="E161" s="3">
+        <v>0</v>
+      </c>
+      <c r="F161" s="3">
+        <v>40</v>
+      </c>
+      <c r="I161" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J161" s="8">
+        <f t="shared" si="15"/>
+        <v>4.125</v>
+      </c>
+    </row>
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A162" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C162" s="3">
+        <v>9</v>
+      </c>
+      <c r="D162" s="3">
+        <v>75</v>
+      </c>
+      <c r="E162" s="3">
+        <v>0</v>
+      </c>
+      <c r="F162" s="3">
+        <v>40</v>
+      </c>
+      <c r="G162" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="I162" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J162" s="8">
+        <f t="shared" si="15"/>
+        <v>4.125</v>
+      </c>
+      <c r="K162" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L162" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A163" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C163" s="5">
+        <v>10</v>
+      </c>
+      <c r="D163" s="3">
+        <v>75</v>
+      </c>
+      <c r="E163" s="3">
+        <v>0</v>
+      </c>
+      <c r="F163" s="3">
+        <v>40</v>
+      </c>
+      <c r="I163" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J163" s="8">
+        <f t="shared" si="15"/>
+        <v>4.125</v>
+      </c>
+      <c r="K163" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L163" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A164" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C164" s="3">
+        <v>11</v>
+      </c>
+      <c r="D164" s="3">
+        <v>75</v>
+      </c>
+      <c r="E164" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="F164" s="3">
+        <v>40</v>
+      </c>
+      <c r="I164" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.375</v>
+      </c>
+      <c r="J164" s="8">
+        <f t="shared" si="15"/>
+        <v>3.75</v>
+      </c>
+    </row>
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A165" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C165" s="5">
+        <v>12</v>
+      </c>
+      <c r="D165" s="3">
+        <v>75</v>
+      </c>
+      <c r="E165" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="F165" s="3">
+        <v>40</v>
+      </c>
+      <c r="I165" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.375</v>
+      </c>
+      <c r="J165" s="8">
+        <f t="shared" si="15"/>
+        <v>3.375</v>
+      </c>
+      <c r="L165" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A166" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C166" s="3">
+        <v>13</v>
+      </c>
+      <c r="D166" s="3">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="E166" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F166" s="3">
+        <v>40</v>
+      </c>
+      <c r="I166" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.68400000000000005</v>
+      </c>
+      <c r="J166" s="8">
+        <f t="shared" si="15"/>
+        <v>2.6909999999999998</v>
+      </c>
+      <c r="L166" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A167" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C167" s="3">
+        <v>14</v>
+      </c>
+      <c r="D167" s="3">
+        <v>60</v>
+      </c>
+      <c r="E167" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F167" s="3">
+        <v>40</v>
+      </c>
+      <c r="I167" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.6</v>
+      </c>
+      <c r="J167" s="8">
+        <f t="shared" si="15"/>
+        <v>2.0909999999999997</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A168" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C168" s="5">
+        <v>15</v>
+      </c>
+      <c r="D168" s="3">
+        <v>60</v>
+      </c>
+      <c r="E168" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F168" s="3">
+        <v>40</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I168" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.6</v>
+      </c>
+      <c r="J168" s="8">
+        <f t="shared" si="15"/>
+        <v>1.4909999999999997</v>
+      </c>
+      <c r="K168" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L168" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A169" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C169" s="3">
+        <v>16</v>
+      </c>
+      <c r="D169" s="3">
+        <v>50</v>
+      </c>
+      <c r="E169" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="F169" s="3">
+        <v>40</v>
+      </c>
+      <c r="G169" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I169" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.25</v>
+      </c>
+      <c r="J169" s="8">
+        <f t="shared" si="15"/>
+        <v>1.2409999999999997</v>
+      </c>
+      <c r="K169" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="L169" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A170" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C170" s="5">
+        <v>17</v>
+      </c>
+      <c r="D170" s="3">
+        <v>200</v>
+      </c>
+      <c r="E170" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="F170" s="3">
+        <v>55</v>
+      </c>
+      <c r="I170" s="8">
+        <f>E170*D170/100</f>
+        <v>-1</v>
+      </c>
+      <c r="J170" s="8">
+        <f t="shared" si="15"/>
+        <v>0.24099999999999966</v>
+      </c>
+    </row>
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A171" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C171" s="3">
+        <v>18</v>
+      </c>
+      <c r="D171" s="3">
+        <v>400</v>
+      </c>
+      <c r="E171" s="3">
+        <f>-100*0.241/400</f>
+        <v>-6.0249999999999998E-2</v>
+      </c>
+      <c r="F171" s="3">
+        <v>70</v>
+      </c>
+      <c r="I171" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.24099999999999999</v>
+      </c>
+      <c r="J171" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A172" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C172" s="3">
+        <v>19</v>
+      </c>
+      <c r="D172" s="3">
+        <v>400</v>
+      </c>
+      <c r="E172" s="3">
+        <v>0</v>
+      </c>
+      <c r="F172" s="3">
+        <v>70</v>
+      </c>
+      <c r="I172" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J172" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A173" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C173" s="5">
+        <v>20</v>
+      </c>
+      <c r="D173" s="3">
+        <v>200</v>
+      </c>
+      <c r="E173" s="3">
+        <v>0</v>
+      </c>
+      <c r="F173" s="3">
+        <v>70</v>
+      </c>
+      <c r="I173" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J173" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="L173" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A174" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C174" s="3">
+        <v>21</v>
+      </c>
+      <c r="D174" s="3">
+        <v>100</v>
+      </c>
+      <c r="E174" s="3">
+        <v>0</v>
+      </c>
+      <c r="F174" s="3">
+        <v>55</v>
+      </c>
+      <c r="G174" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="I174" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J174" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="L174" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A175" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C175" s="5">
+        <v>22</v>
+      </c>
+      <c r="D175" s="3">
+        <v>100</v>
+      </c>
+      <c r="E175" s="3">
+        <v>0</v>
+      </c>
+      <c r="F175" s="3">
+        <v>55</v>
+      </c>
+      <c r="I175" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J175" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A176" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C176" s="3">
+        <v>23</v>
+      </c>
+      <c r="D176" s="3">
+        <v>100</v>
+      </c>
+      <c r="E176" s="3">
+        <v>0</v>
+      </c>
+      <c r="F176" s="3">
+        <v>55</v>
+      </c>
+      <c r="I176" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J176" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="L176" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A177" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C177" s="3">
+        <v>24</v>
+      </c>
+      <c r="D177" s="3">
+        <v>50</v>
+      </c>
+      <c r="E177" s="3">
+        <v>0</v>
+      </c>
+      <c r="F177" s="3">
+        <v>70</v>
+      </c>
+      <c r="G177" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I177" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J177" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="L177" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="178" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A178" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C178" s="5">
+        <v>25</v>
+      </c>
+      <c r="D178" s="3">
+        <v>50</v>
+      </c>
+      <c r="E178" s="3">
+        <v>0</v>
+      </c>
+      <c r="F178" s="3">
+        <v>70</v>
+      </c>
+      <c r="G178" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="I178" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J178" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A179" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C179" s="3">
+        <v>26</v>
+      </c>
+      <c r="D179" s="3">
+        <v>50</v>
+      </c>
+      <c r="E179" s="3">
+        <v>0</v>
+      </c>
+      <c r="F179" s="3">
+        <v>70</v>
+      </c>
+      <c r="G179" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I179" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J179" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A180" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C180" s="5">
+        <v>27</v>
+      </c>
+      <c r="D180" s="3">
+        <v>50</v>
+      </c>
+      <c r="E180" s="3">
+        <v>0</v>
+      </c>
+      <c r="F180" s="3">
+        <v>70</v>
+      </c>
+      <c r="G180" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I180" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J180" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="K180" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A181" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C181" s="3">
+        <v>28</v>
+      </c>
+      <c r="D181" s="3">
+        <v>50</v>
+      </c>
+      <c r="E181" s="3">
+        <v>0</v>
+      </c>
+      <c r="F181" s="3">
+        <v>70</v>
+      </c>
+      <c r="G181" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I181" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J181" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="K181" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A182" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C182" s="3">
+        <v>29</v>
+      </c>
+      <c r="D182" s="3">
+        <v>60</v>
+      </c>
+      <c r="E182" s="3">
+        <v>0</v>
+      </c>
+      <c r="F182" s="3">
+        <v>70</v>
+      </c>
+      <c r="G182" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I182" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J182" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A183" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C183" s="5">
+        <v>30</v>
+      </c>
+      <c r="D183" s="3">
+        <v>60</v>
+      </c>
+      <c r="E183" s="3">
+        <v>0</v>
+      </c>
+      <c r="F183" s="3">
+        <v>70</v>
+      </c>
+      <c r="G183" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I183" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J183" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A184" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C184" s="3">
+        <v>31</v>
+      </c>
+      <c r="D184" s="3">
+        <v>50</v>
+      </c>
+      <c r="E184" s="3">
+        <v>0</v>
+      </c>
+      <c r="F184" s="3">
+        <v>70</v>
+      </c>
+      <c r="G184" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I184" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J184" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A185" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C185" s="5">
+        <v>32</v>
+      </c>
+      <c r="D185" s="3">
+        <v>50</v>
+      </c>
+      <c r="E185" s="3">
+        <v>0</v>
+      </c>
+      <c r="F185" s="3">
+        <v>70</v>
+      </c>
+      <c r="G185" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I185" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J185" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="K185" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A186" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C186" s="3">
+        <v>33</v>
+      </c>
+      <c r="D186" s="3">
+        <v>50</v>
+      </c>
+      <c r="E186" s="3">
+        <v>0</v>
+      </c>
+      <c r="F186" s="3">
+        <v>70</v>
+      </c>
+      <c r="G186" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I186" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J186" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="K186" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A187" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C187" s="3">
+        <v>34</v>
+      </c>
+      <c r="D187" s="3">
+        <v>50</v>
+      </c>
+      <c r="E187" s="3">
+        <v>0</v>
+      </c>
+      <c r="F187" s="3">
+        <v>70</v>
+      </c>
+      <c r="G187" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I187" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J187" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="188" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A188" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C188" s="5">
+        <v>35</v>
+      </c>
+      <c r="D188" s="3">
+        <v>50</v>
+      </c>
+      <c r="E188" s="3">
+        <v>0</v>
+      </c>
+      <c r="F188" s="3">
+        <v>70</v>
+      </c>
+      <c r="G188" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I188" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J188" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A189" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C189" s="3">
+        <v>36</v>
+      </c>
+      <c r="D189" s="3">
+        <v>50</v>
+      </c>
+      <c r="E189" s="3">
+        <v>0</v>
+      </c>
+      <c r="F189" s="3">
+        <v>70</v>
+      </c>
+      <c r="G189" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I189" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J189" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A190" s="3" t="str">
+        <f>A186</f>
+        <v>Red</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C190" s="3">
+        <v>37</v>
+      </c>
+      <c r="D190" s="3">
+        <v>50</v>
+      </c>
+      <c r="E190" s="3">
+        <v>0</v>
+      </c>
+      <c r="F190" s="3">
+        <v>70</v>
+      </c>
+      <c r="G190" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I190" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J190" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A191" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C191" s="5">
+        <v>38</v>
+      </c>
+      <c r="D191" s="3">
+        <v>50</v>
+      </c>
+      <c r="E191" s="3">
+        <v>0</v>
+      </c>
+      <c r="F191" s="3">
+        <v>70</v>
+      </c>
+      <c r="G191" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I191" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J191" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="K191" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A192" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C192" s="3">
+        <v>39</v>
+      </c>
+      <c r="D192" s="3">
+        <v>50</v>
+      </c>
+      <c r="E192" s="3">
+        <v>0</v>
+      </c>
+      <c r="F192" s="3">
+        <v>70</v>
+      </c>
+      <c r="G192" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I192" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J192" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="K192" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A193" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C193" s="3">
+        <v>40</v>
+      </c>
+      <c r="D193" s="3">
+        <v>60</v>
+      </c>
+      <c r="E193" s="3">
+        <v>0</v>
+      </c>
+      <c r="F193" s="3">
+        <v>70</v>
+      </c>
+      <c r="G193" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I193" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J193" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A194" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C194" s="5">
+        <v>41</v>
+      </c>
+      <c r="D194" s="3">
+        <v>60</v>
+      </c>
+      <c r="E194" s="3">
+        <v>0</v>
+      </c>
+      <c r="F194" s="3">
+        <v>70</v>
+      </c>
+      <c r="G194" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I194" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J194" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A195" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B195" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C195" s="3">
+        <v>42</v>
+      </c>
+      <c r="D195" s="3">
+        <v>50</v>
+      </c>
+      <c r="E195" s="3">
+        <v>0</v>
+      </c>
+      <c r="F195" s="3">
+        <v>70</v>
+      </c>
+      <c r="G195" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I195" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J195" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A196" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B196" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C196" s="3">
+        <v>43</v>
+      </c>
+      <c r="D196" s="3">
+        <v>50</v>
+      </c>
+      <c r="E196" s="3">
+        <v>0</v>
+      </c>
+      <c r="F196" s="3">
+        <v>70</v>
+      </c>
+      <c r="G196" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="I196" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J196" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="K196" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A197" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B197" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C197" s="5">
+        <v>44</v>
+      </c>
+      <c r="D197" s="3">
+        <v>50</v>
+      </c>
+      <c r="E197" s="3">
+        <v>0</v>
+      </c>
+      <c r="F197" s="3">
+        <v>70</v>
+      </c>
+      <c r="G197" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I197" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J197" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="K197" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A198" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B198" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C198" s="3">
+        <v>45</v>
+      </c>
+      <c r="D198" s="3">
+        <v>50</v>
+      </c>
+      <c r="E198" s="3">
+        <v>0</v>
+      </c>
+      <c r="F198" s="3">
+        <v>70</v>
+      </c>
+      <c r="G198" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="I198" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J198" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="L198" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A199" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B199" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C199" s="3">
+        <v>46</v>
+      </c>
+      <c r="D199" s="3">
+        <v>75</v>
+      </c>
+      <c r="E199" s="3">
+        <v>0</v>
+      </c>
+      <c r="F199" s="3">
+        <v>70</v>
+      </c>
+      <c r="G199" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I199" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J199" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="L199" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A200" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B200" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C200" s="5">
+        <v>47</v>
+      </c>
+      <c r="D200" s="3">
+        <v>75</v>
+      </c>
+      <c r="E200" s="3">
+        <v>0</v>
+      </c>
+      <c r="F200" s="3">
+        <v>70</v>
+      </c>
+      <c r="G200" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I200" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J200" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A201" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B201" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C201" s="3">
+        <v>48</v>
+      </c>
+      <c r="D201" s="3">
+        <v>75</v>
+      </c>
+      <c r="E201" s="3">
+        <v>0</v>
+      </c>
+      <c r="F201" s="3">
+        <v>70</v>
+      </c>
+      <c r="G201" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="I201" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J201" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="L201" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A202" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B202" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C202" s="3">
+        <v>49</v>
+      </c>
+      <c r="D202" s="3">
+        <v>50</v>
+      </c>
+      <c r="E202" s="3">
+        <v>0</v>
+      </c>
+      <c r="F202" s="3">
+        <v>60</v>
+      </c>
+      <c r="I202" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J202" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="L202" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A203" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C203" s="5">
+        <v>50</v>
+      </c>
+      <c r="D203" s="3">
+        <v>50</v>
+      </c>
+      <c r="E203" s="3">
+        <v>0</v>
+      </c>
+      <c r="F203" s="3">
+        <v>60</v>
+      </c>
+      <c r="I203" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J203" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A204" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B204" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C204" s="3">
+        <v>51</v>
+      </c>
+      <c r="D204" s="3">
+        <v>50</v>
+      </c>
+      <c r="E204" s="3">
+        <v>0</v>
+      </c>
+      <c r="F204" s="3">
+        <v>55</v>
+      </c>
+      <c r="I204" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J204" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+    </row>
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A205" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B205" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C205" s="3">
+        <v>52</v>
+      </c>
+      <c r="D205" s="3">
+        <v>43.2</v>
+      </c>
+      <c r="E205" s="3">
+        <v>0</v>
+      </c>
+      <c r="F205" s="3">
+        <v>55</v>
+      </c>
+      <c r="G205" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I205" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J205" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="K205" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A206" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B206" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C206" s="5">
+        <v>53</v>
+      </c>
+      <c r="D206" s="3">
+        <v>50</v>
+      </c>
+      <c r="E206" s="3">
+        <v>0</v>
+      </c>
+      <c r="F206" s="3">
+        <v>55</v>
+      </c>
+      <c r="I206" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J206" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="K206" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A207" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C207" s="3">
+        <v>54</v>
+      </c>
+      <c r="D207" s="3">
+        <v>50</v>
+      </c>
+      <c r="E207" s="3">
+        <v>0</v>
+      </c>
+      <c r="F207" s="3">
+        <v>55</v>
+      </c>
+      <c r="I207" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J207" s="8">
+        <f t="shared" si="15"/>
+        <v>-3.3306690738754696E-16</v>
+      </c>
+      <c r="L207" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A208" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C208" s="3">
+        <v>55</v>
+      </c>
+      <c r="D208" s="3">
+        <v>75</v>
+      </c>
+      <c r="E208" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F208" s="3">
+        <v>55</v>
+      </c>
+      <c r="I208" s="8">
+        <f t="shared" si="13"/>
+        <v>0.375</v>
+      </c>
+      <c r="J208" s="8">
+        <f t="shared" si="15"/>
+        <v>0.37499999999999967</v>
+      </c>
+      <c r="L208" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A209" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B209" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C209" s="5">
+        <v>56</v>
+      </c>
+      <c r="D209" s="3">
+        <v>75</v>
+      </c>
+      <c r="E209" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F209" s="3">
+        <v>55</v>
+      </c>
+      <c r="I209" s="8">
+        <f t="shared" si="13"/>
+        <v>0.375</v>
+      </c>
+      <c r="J209" s="8">
+        <f t="shared" si="15"/>
+        <v>0.74999999999999967</v>
+      </c>
+    </row>
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A210" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B210" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C210" s="3">
+        <v>57</v>
+      </c>
+      <c r="D210" s="3">
+        <v>75</v>
+      </c>
+      <c r="E210" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F210" s="3">
+        <v>55</v>
+      </c>
+      <c r="I210" s="8">
+        <f t="shared" si="13"/>
+        <v>0.375</v>
+      </c>
+      <c r="J210" s="8">
+        <f t="shared" si="15"/>
+        <v>1.1249999999999996</v>
+      </c>
+      <c r="L210" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A211" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B211" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C211" s="3">
+        <v>58</v>
+      </c>
+      <c r="D211" s="3">
+        <v>75</v>
+      </c>
+      <c r="E211" s="3">
+        <v>1</v>
+      </c>
+      <c r="F211" s="3">
+        <v>55</v>
+      </c>
+      <c r="I211" s="8">
+        <f t="shared" si="13"/>
+        <v>0.75</v>
+      </c>
+      <c r="J211" s="8">
+        <f t="shared" si="15"/>
+        <v>1.8749999999999996</v>
+      </c>
+      <c r="L211" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A212" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B212" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C212" s="5">
+        <v>59</v>
+      </c>
+      <c r="D212" s="3">
+        <v>75</v>
+      </c>
+      <c r="E212" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="F212" s="3">
+        <v>55</v>
+      </c>
+      <c r="I212" s="8">
+        <f t="shared" si="13"/>
+        <v>0.375</v>
+      </c>
+      <c r="J212" s="8">
+        <f t="shared" si="15"/>
+        <v>2.2499999999999996</v>
+      </c>
+    </row>
+    <row r="213" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A213" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B213" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C213" s="3">
+        <v>60</v>
+      </c>
+      <c r="D213" s="3">
+        <v>75</v>
+      </c>
+      <c r="E213" s="3">
+        <v>0</v>
+      </c>
+      <c r="F213" s="3">
+        <v>55</v>
+      </c>
+      <c r="G213" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="I213" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J213" s="8">
+        <f t="shared" si="15"/>
+        <v>2.2499999999999996</v>
+      </c>
+      <c r="L213" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A214" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B214" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C214" s="3">
+        <v>61</v>
+      </c>
+      <c r="D214" s="3">
+        <v>75</v>
+      </c>
+      <c r="E214" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="F214" s="3">
+        <v>55</v>
+      </c>
+      <c r="I214" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.375</v>
+      </c>
+      <c r="J214" s="8">
+        <f t="shared" si="15"/>
+        <v>1.8749999999999996</v>
+      </c>
+      <c r="L214" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A215" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C215" s="5">
+        <v>62</v>
+      </c>
+      <c r="D215" s="3">
+        <v>75</v>
+      </c>
+      <c r="E215" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F215" s="3">
+        <v>55</v>
+      </c>
+      <c r="I215" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.75</v>
+      </c>
+      <c r="J215" s="8">
+        <f t="shared" si="15"/>
+        <v>1.1249999999999996</v>
+      </c>
+    </row>
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B216" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C216" s="3">
+        <v>63</v>
+      </c>
+      <c r="D216" s="3">
+        <v>75</v>
+      </c>
+      <c r="E216" s="3">
+        <v>-1</v>
+      </c>
+      <c r="F216" s="3">
+        <v>55</v>
+      </c>
+      <c r="I216" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.75</v>
+      </c>
+      <c r="J216" s="8">
+        <f t="shared" si="15"/>
+        <v>0.37499999999999956</v>
+      </c>
+      <c r="L216" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A217" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C217" s="3">
+        <v>64</v>
+      </c>
+      <c r="D217" s="3">
+        <v>75</v>
+      </c>
+      <c r="E217" s="3">
+        <v>-0.5</v>
+      </c>
+      <c r="F217" s="3">
+        <v>55</v>
+      </c>
+      <c r="I217" s="8">
+        <f t="shared" si="13"/>
+        <v>-0.375</v>
+      </c>
+      <c r="J217" s="8">
+        <f t="shared" si="15"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="L217" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C218" s="5">
+        <v>65</v>
+      </c>
+      <c r="D218" s="3">
+        <v>75</v>
+      </c>
+      <c r="E218" s="3">
+        <v>0</v>
+      </c>
+      <c r="F218" s="3">
+        <v>55</v>
+      </c>
+      <c r="I218" s="8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J218" s="8">
+        <f t="shared" si="15"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+    </row>
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="str">
+        <f t="shared" si="14"/>
+        <v>Red</v>
+      </c>
+      <c r="B219" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C219" s="3">
+        <v>66</v>
+      </c>
+      <c r="D219" s="3">
+        <v>75</v>
+      </c>
+      <c r="E219" s="3">
+        <v>0</v>
+      </c>
+      <c r="F219" s="3">
+        <v>55</v>
+      </c>
+      <c r="I219" s="8">
+        <f t="shared" ref="I219:I230" si="16">E219*D219/100</f>
+        <v>0</v>
+      </c>
+      <c r="J219" s="8">
+        <f t="shared" si="15"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="K219" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="L219" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="str">
+        <f t="shared" ref="A220:A229" si="17">A219</f>
+        <v>Red</v>
+      </c>
+      <c r="B220" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C220" s="3">
+        <v>67</v>
+      </c>
+      <c r="D220" s="3">
+        <v>50</v>
+      </c>
+      <c r="E220" s="3">
+        <v>0</v>
+      </c>
+      <c r="F220" s="3">
+        <v>55</v>
+      </c>
+      <c r="G220" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I220" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J220" s="8">
+        <f t="shared" ref="J220:J230" si="18">I220+J219</f>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="K220" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="L220" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>Red</v>
+      </c>
+      <c r="B221" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C221" s="5">
+        <v>68</v>
+      </c>
+      <c r="D221" s="3">
+        <v>50</v>
+      </c>
+      <c r="E221" s="3">
+        <v>0</v>
+      </c>
+      <c r="F221" s="3">
+        <v>55</v>
+      </c>
+      <c r="G221" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I221" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J221" s="8">
+        <f t="shared" si="18"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="L221" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>Red</v>
+      </c>
+      <c r="B222" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C222" s="3">
+        <v>69</v>
+      </c>
+      <c r="D222" s="3">
+        <v>50</v>
+      </c>
+      <c r="E222" s="3">
+        <v>0</v>
+      </c>
+      <c r="F222" s="3">
+        <v>55</v>
+      </c>
+      <c r="G222" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I222" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J222" s="8">
+        <f t="shared" si="18"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+    </row>
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>Red</v>
+      </c>
+      <c r="B223" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C223" s="3">
+        <v>70</v>
+      </c>
+      <c r="D223" s="3">
+        <v>50</v>
+      </c>
+      <c r="E223" s="3">
+        <v>0</v>
+      </c>
+      <c r="F223" s="3">
+        <v>55</v>
+      </c>
+      <c r="G223" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I223" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J223" s="8">
+        <f t="shared" si="18"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="L223" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A224" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>Red</v>
+      </c>
+      <c r="B224" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C224" s="5">
+        <v>71</v>
+      </c>
+      <c r="D224" s="3">
+        <v>50</v>
+      </c>
+      <c r="E224" s="3">
+        <v>0</v>
+      </c>
+      <c r="F224" s="3">
+        <v>55</v>
+      </c>
+      <c r="G224" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I224" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J224" s="8">
+        <f t="shared" si="18"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="K224" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="L224" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A225" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>Red</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C225" s="3">
+        <v>72</v>
+      </c>
+      <c r="D225" s="3">
+        <v>50</v>
+      </c>
+      <c r="E225" s="3">
+        <v>0</v>
+      </c>
+      <c r="F225" s="3">
+        <v>55</v>
+      </c>
+      <c r="G225" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I225" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J225" s="8">
+        <f t="shared" si="18"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="K225" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="L225" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A226" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>Red</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C226" s="3">
+        <v>73</v>
+      </c>
+      <c r="D226" s="3">
+        <v>50</v>
+      </c>
+      <c r="E226" s="3">
+        <v>0</v>
+      </c>
+      <c r="F226" s="3">
+        <v>55</v>
+      </c>
+      <c r="G226" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I226" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J226" s="8">
+        <f t="shared" si="18"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="L226" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A227" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>Red</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C227" s="5">
+        <v>74</v>
+      </c>
+      <c r="D227" s="3">
+        <v>50</v>
+      </c>
+      <c r="E227" s="3">
+        <v>0</v>
+      </c>
+      <c r="F227" s="3">
+        <v>55</v>
+      </c>
+      <c r="G227" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I227" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J227" s="8">
+        <f t="shared" si="18"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+    </row>
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A228" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>Red</v>
+      </c>
+      <c r="B228" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C228" s="3">
+        <v>75</v>
+      </c>
+      <c r="D228" s="3">
+        <v>50</v>
+      </c>
+      <c r="E228" s="3">
+        <v>0</v>
+      </c>
+      <c r="F228" s="3">
+        <v>55</v>
+      </c>
+      <c r="G228" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I228" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J228" s="8">
+        <f t="shared" si="18"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="L228" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A229" s="3" t="str">
+        <f t="shared" si="17"/>
+        <v>Red</v>
+      </c>
+      <c r="B229" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C229" s="3">
+        <v>76</v>
+      </c>
+      <c r="D229" s="3">
+        <v>50</v>
+      </c>
+      <c r="E229" s="3">
+        <v>0</v>
+      </c>
+      <c r="F229" s="3">
+        <v>55</v>
+      </c>
+      <c r="G229" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I229" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J229" s="8">
+        <f t="shared" si="18"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="K229" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="L229" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A230" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C230" s="5">
+        <v>77</v>
+      </c>
+      <c r="D230" s="3">
+        <v>50</v>
+      </c>
+      <c r="E230" s="3">
+        <v>0</v>
+      </c>
+      <c r="F230" s="3">
+        <v>35</v>
+      </c>
+      <c r="I230" s="8">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="J230" s="8">
+        <f t="shared" si="18"/>
+        <v>-4.4408920985006262E-16</v>
+      </c>
+      <c r="K230" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="L230" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Block functionality update, speedAndAuthority update Added functioning isUnderground to Block object when loading from db. Added updateSpeedAndAuthority() method (called by TrackController) Added functional isFrom/ToYard on blocks.
</commit_message>
<xml_diff>
--- a/TrainProject/Excel Files/TrackLayout.xlsx
+++ b/TrainProject/Excel Files/TrackLayout.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7530" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Red Line" sheetId="1" r:id="rId1"/>
@@ -3527,8 +3527,8 @@
   <dimension ref="A1:L230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E169" sqref="E169"/>
+      <pane ySplit="1" topLeftCell="A68" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added StationBeacons (hard coded)
</commit_message>
<xml_diff>
--- a/TrainProject/Excel Files/TrackLayout.xlsx
+++ b/TrainProject/Excel Files/TrackLayout.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="661" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="660" uniqueCount="91">
   <si>
     <t>Block Number</t>
   </si>
@@ -289,10 +289,10 @@
     <t>STATION; PENN STATION; UNDERGROUND</t>
   </si>
   <si>
-    <t>STATION; HERRON AVE</t>
+    <t>STATION; SHADYSIDE</t>
   </si>
   <si>
-    <t>STATION; SHADYSIDE</t>
+    <t>SWITCH; STATION; HERRON AVE</t>
   </si>
 </sst>
 </file>
@@ -3542,8 +3542,8 @@
   <dimension ref="A1:L230"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
+      <pane ySplit="1" topLeftCell="A167" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H169" sqref="H169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -8618,7 +8618,7 @@
         <v>40</v>
       </c>
       <c r="G160" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I160" s="8">
         <f t="shared" si="13"/>
@@ -8876,9 +8876,6 @@
       <c r="F168" s="3">
         <v>40</v>
       </c>
-      <c r="G168" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="I168" s="8">
         <f t="shared" si="13"/>
         <v>-0.6</v>
@@ -8894,7 +8891,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="str">
         <f t="shared" si="14"/>
         <v>Red</v>
@@ -8915,7 +8912,7 @@
         <v>40</v>
       </c>
       <c r="G169" s="7" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="I169" s="8">
         <f t="shared" si="13"/>

</xml_diff>